<commit_message>
practica3 fixed initial bug
</commit_message>
<xml_diff>
--- a/CSV/ESTUDIO.xlsx
+++ b/CSV/ESTUDIO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\izana\Documents\GitHub\SEA\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626ADEFD-EF57-4BCB-900E-A4A85442BB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B0D2A5-42F3-475F-BECA-3A9464CB9A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{58D07043-2F25-489D-B121-BB5405FD76E7}"/>
   </bookViews>
@@ -237,13 +237,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -252,8 +246,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -370,10 +370,10 @@
       <xdr:rowOff>166254</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>263632</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>62825</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>348823</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>96982</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -397,7 +397,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13009418" y="2687781"/>
-          <a:ext cx="9019705" cy="5119735"/>
+          <a:ext cx="9714496" cy="5514110"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -708,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCC3A2C-C8C5-4B85-BFEF-834990F9E678}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,10 +735,10 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
@@ -840,93 +840,93 @@
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F17" t="s">
@@ -934,118 +934,118 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="F18" s="6" t="s">
+      <c r="D18" s="4"/>
+      <c r="F18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="6"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="F19" s="7" t="s">
+      <c r="D19" s="5"/>
+      <c r="F19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="7"/>
+      <c r="G19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="F20" s="7" t="s">
+      <c r="D20" s="5"/>
+      <c r="F20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="7"/>
+      <c r="G20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="F21" s="7" t="s">
+      <c r="D21" s="5"/>
+      <c r="F21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="7"/>
+      <c r="G21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="F22" s="7" t="s">
+      <c r="D22" s="5"/>
+      <c r="F22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="7"/>
+      <c r="G22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="F23" s="7" t="s">
+      <c r="D23" s="5"/>
+      <c r="F23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H23" s="7"/>
+      <c r="H23" s="5"/>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
@@ -1056,77 +1056,77 @@
       </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F40" s="7" t="s">
+      <c r="F40" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F41" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F42" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="F43" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F44" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="6" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
practica 3 finished, subject nearly passed
</commit_message>
<xml_diff>
--- a/CSV/ESTUDIO.xlsx
+++ b/CSV/ESTUDIO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\izana\Documents\GitHub\SEA\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B0D2A5-42F3-475F-BECA-3A9464CB9A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B21745-4DA7-4C5F-8188-C39E6BD2811A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{58D07043-2F25-489D-B121-BB5405FD76E7}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{58D07043-2F25-489D-B121-BB5405FD76E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="36">
   <si>
     <t>Tabla estado</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>0010 0011</t>
+  </si>
+  <si>
+    <t>101 (F)</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>0101</t>
   </si>
 </sst>
 </file>
@@ -176,7 +185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -225,11 +234,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -254,6 +274,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -365,15 +388,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>387927</xdr:colOff>
+      <xdr:colOff>387926</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>166254</xdr:rowOff>
+      <xdr:rowOff>166253</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>348823</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>96982</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>33941</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>41562</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -396,8 +419,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13009418" y="2687781"/>
-          <a:ext cx="9714496" cy="5514110"/>
+          <a:off x="13009417" y="2687780"/>
+          <a:ext cx="11838015" cy="6719455"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -706,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCC3A2C-C8C5-4B85-BFEF-834990F9E678}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:AV49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+    <sheetView tabSelected="1" topLeftCell="AL22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="AP29" sqref="AP29:AQ29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -925,7 +948,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>23</v>
       </c>
@@ -933,7 +956,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
@@ -952,7 +975,7 @@
       </c>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>12</v>
       </c>
@@ -971,7 +994,7 @@
       </c>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>11</v>
       </c>
@@ -990,7 +1013,7 @@
       </c>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>10</v>
       </c>
@@ -1009,7 +1032,7 @@
       </c>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>13</v>
       </c>
@@ -1027,8 +1050,14 @@
         <v>16</v>
       </c>
       <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="AO22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="AT22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>14</v>
       </c>
@@ -1046,8 +1075,185 @@
         <v>17</v>
       </c>
       <c r="H23" s="5"/>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="AO23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AQ23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AR23" s="4"/>
+      <c r="AT23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AU23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV23" s="4"/>
+    </row>
+    <row r="24" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AO24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR24" s="5"/>
+      <c r="AT24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV24" s="5"/>
+    </row>
+    <row r="25" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AO25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AP25" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AQ25" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR25" s="5"/>
+      <c r="AT25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV25" s="5"/>
+    </row>
+    <row r="26" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AO26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AP26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AR26" s="5"/>
+      <c r="AT26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AU26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV26" s="5"/>
+    </row>
+    <row r="27" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AO27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR27" s="5"/>
+      <c r="AT27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV27" s="5"/>
+    </row>
+    <row r="28" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AO28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP28" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR28" s="5"/>
+      <c r="AT28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV28" s="5"/>
+    </row>
+    <row r="29" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="AO29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AU29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="3:43" x14ac:dyDescent="0.3">
+      <c r="AP33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ33" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="3:43" x14ac:dyDescent="0.3">
+      <c r="AP34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ34" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="3:43" x14ac:dyDescent="0.3">
+      <c r="AP35" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AQ35" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="3:43" x14ac:dyDescent="0.3">
+      <c r="AP36" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ36" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="3:43" x14ac:dyDescent="0.3">
+      <c r="AP37" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ37" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="3:43" x14ac:dyDescent="0.3">
+      <c r="AP38" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AQ38" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="3:43" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
         <v>23</v>
       </c>
@@ -1055,7 +1261,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:43" x14ac:dyDescent="0.3">
       <c r="C40" s="5" t="s">
         <v>26</v>
       </c>
@@ -1066,7 +1272,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:43" x14ac:dyDescent="0.3">
       <c r="C41" s="5" t="s">
         <v>27</v>
       </c>
@@ -1077,7 +1283,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:43" x14ac:dyDescent="0.3">
       <c r="C42" s="5" t="s">
         <v>27</v>
       </c>
@@ -1088,7 +1294,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:43" x14ac:dyDescent="0.3">
       <c r="C43" s="5" t="s">
         <v>28</v>
       </c>
@@ -1099,7 +1305,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:43" x14ac:dyDescent="0.3">
       <c r="C44" s="5" t="s">
         <v>27</v>
       </c>
@@ -1110,17 +1316,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:43" x14ac:dyDescent="0.3">
       <c r="C46" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:43" x14ac:dyDescent="0.3">
       <c r="C47" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:43" x14ac:dyDescent="0.3">
       <c r="C48" s="6" t="s">
         <v>32</v>
       </c>

</xml_diff>